<commit_message>
added spectral values 2
</commit_message>
<xml_diff>
--- a/tp1/specradius_values.xlsx
+++ b/tp1/specradius_values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nestor\Desktop\tp1numerico\tp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3965D34C-D0C4-412D-BEF4-5559D98067D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B143270-ABFC-408F-ABE9-7A74A8B79DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>N = 4</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>s</t>
-  </si>
-  <si>
-    <t>ln(s)</t>
   </si>
 </sst>
 </file>
@@ -207,10 +204,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,7 +715,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Logaritmo natural del radio espectral en función de w para N = 32</a:t>
+              <a:t>Radio espectral en función de w para N = 32</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -767,7 +764,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ln(s)</c:v>
+                  <c:v>s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -875,67 +872,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>386.01799999999997</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>385.56900000000002</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>384.95800000000003</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>384.51400000000001</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>384.69200000000001</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>386.065</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>377.25299999999999</c:v>
+                  <c:v>0.89800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>382.517</c:v>
+                  <c:v>0.89800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>377.71499999999997</c:v>
+                  <c:v>0.89600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>375.47199999999998</c:v>
+                  <c:v>0.89400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>376.53199999999998</c:v>
+                  <c:v>0.89100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>364.839</c:v>
+                  <c:v>0.88600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>374.12700000000001</c:v>
+                  <c:v>0.88200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>369.67099999999999</c:v>
+                  <c:v>0.876</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>369.65</c:v>
+                  <c:v>0.86799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>346.69600000000003</c:v>
+                  <c:v>0.85699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>335.41199999999998</c:v>
+                  <c:v>0.84799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>337.85899999999998</c:v>
+                  <c:v>0.84799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>361.86599999999999</c:v>
+                  <c:v>0.85599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>382.25400000000002</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>476.209</c:v>
+                  <c:v>0.93300000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2591,8 +2588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,7 +2621,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2638,7 +2635,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="5">
-        <v>386.01799999999997</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2652,7 +2649,7 @@
         <v>1.05</v>
       </c>
       <c r="E4" s="7">
-        <v>385.56900000000002</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2666,7 +2663,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E5" s="5">
-        <v>384.95800000000003</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2680,7 +2677,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="E6" s="7">
-        <v>384.51400000000001</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2694,7 +2691,7 @@
         <v>1.2</v>
       </c>
       <c r="E7" s="5">
-        <v>384.69200000000001</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2708,7 +2705,7 @@
         <v>1.25</v>
       </c>
       <c r="E8" s="7">
-        <v>386.065</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2722,7 +2719,7 @@
         <v>1.3</v>
       </c>
       <c r="E9" s="5">
-        <v>377.25299999999999</v>
+        <v>0.89800000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2736,7 +2733,7 @@
         <v>1350</v>
       </c>
       <c r="E10" s="7">
-        <v>382.517</v>
+        <v>0.89800000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2750,7 +2747,7 @@
         <v>1.4</v>
       </c>
       <c r="E11" s="5">
-        <v>377.71499999999997</v>
+        <v>0.89600000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2764,7 +2761,7 @@
         <v>1450</v>
       </c>
       <c r="E12" s="7">
-        <v>375.47199999999998</v>
+        <v>0.89400000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2778,7 +2775,7 @@
         <v>1.5</v>
       </c>
       <c r="E13" s="5">
-        <v>376.53199999999998</v>
+        <v>0.89100000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2792,7 +2789,7 @@
         <v>1.55</v>
       </c>
       <c r="E14" s="7">
-        <v>364.839</v>
+        <v>0.88600000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2806,7 +2803,7 @@
         <v>1.6</v>
       </c>
       <c r="E15" s="5">
-        <v>374.12700000000001</v>
+        <v>0.88200000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2820,7 +2817,7 @@
         <v>1.65</v>
       </c>
       <c r="E16" s="7">
-        <v>369.67099999999999</v>
+        <v>0.876</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2834,7 +2831,7 @@
         <v>1.7</v>
       </c>
       <c r="E17" s="5">
-        <v>369.65</v>
+        <v>0.86799999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2848,7 +2845,7 @@
         <v>1.75</v>
       </c>
       <c r="E18" s="7">
-        <v>346.69600000000003</v>
+        <v>0.85699999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2862,7 +2859,7 @@
         <v>1.8</v>
       </c>
       <c r="E19" s="5">
-        <v>335.41199999999998</v>
+        <v>0.84799999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2876,7 +2873,7 @@
         <v>1.821</v>
       </c>
       <c r="E20" s="7">
-        <v>337.85899999999998</v>
+        <v>0.84799999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2890,7 +2887,7 @@
         <v>1.85</v>
       </c>
       <c r="E21" s="5">
-        <v>361.86599999999999</v>
+        <v>0.85599999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2904,7 +2901,7 @@
         <v>1.9</v>
       </c>
       <c r="E22" s="7">
-        <v>382.25400000000002</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2918,7 +2915,7 @@
         <v>1.95</v>
       </c>
       <c r="E23" s="5">
-        <v>476.209</v>
+        <v>0.93300000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>